<commit_message>
update bom with links
</commit_message>
<xml_diff>
--- a/Documents/RAFbom.xlsx
+++ b/Documents/RAFbom.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zua691/github/RAFLauncher/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zua691/github/RAF/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140" tabRatio="500"/>
+    <workbookView xWindow="-36940" yWindow="-3460" windowWidth="28800" windowHeight="16140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="RAFbom" sheetId="1" r:id="rId1"/>
@@ -28,32 +28,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Per student BOM</t>
   </si>
   <si>
-    <t>Arduino</t>
-  </si>
-  <si>
-    <t>ArduLauncher shield</t>
-  </si>
-  <si>
-    <t>Solenoid power supply (not needed if we go with 5V servos</t>
-  </si>
-  <si>
     <t>USB cable for Arduino</t>
   </si>
   <si>
     <t>2 ft of air tubing</t>
   </si>
   <si>
-    <t>Barrel (3 ml Syringe)</t>
-  </si>
-  <si>
-    <t>Pan Tilt Mechanism parts</t>
-  </si>
-  <si>
     <t>Hardware for pan tilt mechanism.</t>
   </si>
   <si>
@@ -63,9 +48,6 @@
     <t>Soda bottle for air tank</t>
   </si>
   <si>
-    <t>30 ml syringe</t>
-  </si>
-  <si>
     <t>2x one way valves</t>
   </si>
   <si>
@@ -112,13 +94,73 @@
   </si>
   <si>
     <t>Gas solenoid valve</t>
+  </si>
+  <si>
+    <t>Arduino Uno R3 (make sure it has a 16u2)</t>
+  </si>
+  <si>
+    <t>9V 2.5A or greater power supply</t>
+  </si>
+  <si>
+    <t>RAF Shield</t>
+  </si>
+  <si>
+    <t>Supplier link</t>
+  </si>
+  <si>
+    <t>http://www.microcenter.com/product/486544/Uno_R3_MainBoard</t>
+  </si>
+  <si>
+    <t>https://hobbyking.com/en_us/hobbykingtm-hk15138-standard-analog-servo-4-3kg-0-17sec-38g.html</t>
+  </si>
+  <si>
+    <t>http://www.lynxmotion.com/p-288-lynx-b-pan-and-tilt-kit-black-anodized-no-servos.aspx</t>
+  </si>
+  <si>
+    <t>3D printed barrel holder</t>
+  </si>
+  <si>
+    <t>3D printed servo base</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/2Pcs-Aquarium-Bottle-Caps-for-DIY-CO2-System-Kit-Generator-Part-Live-Plants-Diffuser-Air-Letter/32568982068.html</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/300-Pieces-Compatible-N-Strike-Universal-Accessories/dp/B01IQAMN4G/</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/10x-Aquarium-One-Way-Check-Valve-Non-Return-Fish-Tank-Air-Pump-CO2-System-Red/32705403205.html</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/UXCELL-Auto-Car-3Mm-Inner-Dia-T-Piece-Tube-Hose-Pipe-Tee-Connector-Fittings-White-50Pcs/32801628670.html</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/free-shipping-100pcs-lot-1-8inch-Barb-Female-Luer-Tapered-Syringe-Fitting-polyprop-Luer-Lock-Tapered/32822131398.html?spm=2114.search0104.3.1.9OLhnr&amp;ws_ab_test=searchweb0_0,searchweb201602_5_10152_5560013_10065_10151_10130_10068_10344_10342_10343_10340_10341_10307_10060_10155_10154_10056_10055_5370013_10054_10059_10534_10533_10532_100031_10099_10338_10339_10103_10102_5580013_10052_10053_10107_10050_10142_10051_10324_10325_10084_513_10083_10080_10082_10081_10178_10110_10111_10112_5590013_10113_10114_143_10312_10314_5570013_10078_10079_10073,searchweb201603_2,ppcSwitch_2&amp;btsid=c7f45d3b-ea8b-430d-b965-d652c82e57e3&amp;algo_expid=ed763a4b-153f-4dc6-8288-40b75d67cfc9-0&amp;algo_pvid=ed763a4b-153f-4dc6-8288-40b75d67cfc9</t>
+  </si>
+  <si>
+    <t>electric air pump</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/DC-6V-Mini-Air-Pump-Motor-for-Aquarium-Tank-Oxygen-Circulate/32794737297.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> or 30 ml syringe</t>
+  </si>
+  <si>
+    <t>Barrel (5 ml Syringe)</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/100PCS-New-2016-Reusable-5ML-Large-Big-Plastic-Hydroponics-Nutrient-Measuring-Syringe/32617036933.html</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/10PCS-LOT-DC12V-Solenoid-valve-Mini-Micro-electric-Water-Gas-valve-Discouraged-Normally-closed-6-8/32796259307.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -130,6 +172,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -152,10 +202,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -164,8 +215,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -441,187 +494,244 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="3"/>
-    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="53.6640625" customWidth="1"/>
+    <col min="3" max="3" width="55.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
-        <v>1</v>
-      </c>
       <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>1</v>
       </c>
       <c r="B7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>1</v>
       </c>
       <c r="B19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" t="s">
-        <v>21</v>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C12" r:id="rId1"/>
+    <hyperlink ref="C9" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -641,10 +751,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -652,7 +762,7 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -660,7 +770,7 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>